<commit_message>
0704: cal fct rtn
</commit_message>
<xml_diff>
--- a/BarraPCA/access_barra.xlsx
+++ b/BarraPCA/access_barra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\barra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winst\Nutstore\1\我的坚果云\XJIntern\PyCharmProject\BarraPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9068DD-B20B-4F0B-9C51-BA54336318B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965156C6-5BAD-43B9-80E8-61699FDDD2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4236" yWindow="1824" windowWidth="16824" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="636" yWindow="1080" windowWidth="15576" windowHeight="11868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="access_target" sheetId="1" r:id="rId1"/>
@@ -1029,9 +1029,6 @@
     <filterColumn colId="9" hiddenButton="1"/>
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K1">
-    <sortCondition descending="1" ref="K1"/>
-  </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{E9890D40-424B-4B70-AAA7-10D4D4898842}" name="UPDATE" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{773C700A-01DE-4AA2-927A-741A277DAEE2}" name="SERVER" dataDxfId="9"/>
@@ -1350,7 +1347,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>

</xml_diff>